<commit_message>
Update Excel template with new field instructions
</commit_message>
<xml_diff>
--- a/public/data/template.xlsx
+++ b/public/data/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\CascadeProjects\excel-mobile-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEA81ED-5BA1-4EB0-8D59-A6871D4FC80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E34EE9-1E27-4916-9727-67A962DD889B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,27 +73,18 @@
     <t>Check FOD</t>
   </si>
   <si>
-    <t>Check RAMP to prevent FOD.</t>
-  </si>
-  <si>
     <t>Night serveillance</t>
   </si>
   <si>
     <t>Check drain fuel</t>
   </si>
   <si>
-    <t>Check fuel drainage according to the checklist.</t>
-  </si>
-  <si>
     <t>Night surveillance</t>
   </si>
   <si>
     <t>Check OWP feedback</t>
   </si>
   <si>
-    <t>Ensure OWP feedback is fully recorded.</t>
-  </si>
-  <si>
     <t>Check the condition of aircraft covering.</t>
   </si>
   <si>
@@ -109,15 +100,9 @@
     <t>Check engine wash</t>
   </si>
   <si>
-    <t>Ensure engine wash chemicals are used correctly.</t>
-  </si>
-  <si>
     <t>Check cabin</t>
   </si>
   <si>
-    <t>Conduct a general inspection of the cabin, Lavatory, and Galley.</t>
-  </si>
-  <si>
     <t>Check defects ATA 21, 36</t>
   </si>
   <si>
@@ -133,9 +118,6 @@
     <t>Check engine defects</t>
   </si>
   <si>
-    <t>Check for engine failures, leaks, and loose bolts.</t>
-  </si>
-  <si>
     <t>daily/weekly/phase</t>
   </si>
   <si>
@@ -187,9 +169,6 @@
     <t>Check PTS application</t>
   </si>
   <si>
-    <t>Verify compliance with PTS in operations.</t>
-  </si>
-  <si>
     <t>Check GSE maintenance at VTE</t>
   </si>
   <si>
@@ -436,10 +415,41 @@
     <t>Check cargo</t>
   </si>
   <si>
-    <t>Check for damage, leaks, and defects in the cargo.</t>
-  </si>
-  <si>
     <t>Check cover A/C parking/Storage</t>
+  </si>
+  <si>
+    <t>Check RAMP to prevent FOD.
+1. Quan sát việc tuân thủ kiểm tra FOD bãi đậu trước khi tàu đáp và sau khi đưa tàu đi của NVKT.
+2. Croscheck tại các bãi có bảo dưỡng lớn xem team bải dưỡng có tuân thủ quy trình ngăn ngừa FOD hay không?</t>
+  </si>
+  <si>
+    <t>Check fuel drainage according to the checklist.Random check các tàu thực hiện WKLY có được drain fuel theo WKLY checklist hay không?</t>
+  </si>
+  <si>
+    <t>Ensure OWP feedback is fully recorded.Có thể kiểm tra OWP feedback của ngày hôm trước, với các tiêu chí:
+        a. Các WO từ chối phải có lí do rõ ràng và được sự xác nhận từ MOC.
+        b. Thông tin daily check phải được điền đầy đủ.
+        c. Các WO được thực hiện phải ghi nhận số chứng chỉ của NVKT rõ ràng.</t>
+  </si>
+  <si>
+    <t>Check for damage, leaks, and defects in the cargo.
+a. Kiểm tra các dấu hiệu mục của buồng hàng - đặc biệt là khu vực quanh mép buồng hàng và cửa buồng hàng.
+        b. Kiểm tra tình trạng TDP.
+        c. Kiểm tra các tấm linning buồng hàng.</t>
+  </si>
+  <si>
+    <t>Ensure engine wash chemicals are used correctly.Chi tiết kiểm tra:
+        a. Số lượng hóa chất.
+        b. Số lượng lần rửa</t>
+  </si>
+  <si>
+    <t>Conduct a general inspection of the cabin, Lavatory, and Galley. Tăng cường random check áo phao</t>
+  </si>
+  <si>
+    <t>Check for engine failures, leaks, and loose bolts. Tăng cường kiểm tra vị trí Anti-ice access panel</t>
+  </si>
+  <si>
+    <t>Verify compliance with PTS in operations. PTS là chương trình yêu cầu các đơn vị phải hoàn thành phần việc của mình trong khoảng thời gian CỐ ĐỊNH và TỐI ƯU NHẤT đã được thống nhất bằng văn bản. Nhằm duy trì tổng thời gian dừng/nghỉ giữa các chuyến bay TỐI ƯU.</t>
   </si>
 </sst>
 </file>
@@ -964,7 +974,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="15"/>
@@ -1023,10 +1033,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>11</v>
+        <v>126</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -1040,13 +1050,13 @@
       <c r="B3" s="20"/>
       <c r="C3" s="14"/>
       <c r="D3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -1060,13 +1070,13 @@
       <c r="B4" s="17"/>
       <c r="C4" s="14"/>
       <c r="D4" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -1080,13 +1090,13 @@
       <c r="B5" s="17"/>
       <c r="C5" s="14"/>
       <c r="D5" s="18" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -1100,13 +1110,13 @@
       <c r="B6" s="20"/>
       <c r="C6" s="14"/>
       <c r="D6" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -1120,13 +1130,13 @@
       <c r="B7" s="17"/>
       <c r="C7" s="14"/>
       <c r="D7" s="18" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -1140,13 +1150,13 @@
       <c r="B8" s="20"/>
       <c r="C8" s="14"/>
       <c r="D8" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -1160,13 +1170,13 @@
       <c r="B9" s="20"/>
       <c r="C9" s="14"/>
       <c r="D9" s="18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>25</v>
+        <v>131</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1180,13 +1190,13 @@
       <c r="B10" s="20"/>
       <c r="C10" s="14"/>
       <c r="D10" s="18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -1200,13 +1210,13 @@
       <c r="B11" s="20"/>
       <c r="C11" s="14"/>
       <c r="D11" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -1220,13 +1230,13 @@
       <c r="B12" s="20"/>
       <c r="C12" s="14"/>
       <c r="D12" s="18" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -1240,13 +1250,13 @@
       <c r="B13" s="20"/>
       <c r="C13" s="14"/>
       <c r="D13" s="18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -1260,13 +1270,13 @@
       <c r="B14" s="20"/>
       <c r="C14" s="14"/>
       <c r="D14" s="18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -1280,13 +1290,13 @@
       <c r="B15" s="20"/>
       <c r="C15" s="14"/>
       <c r="D15" s="18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -1300,13 +1310,13 @@
       <c r="B16" s="20"/>
       <c r="C16" s="14"/>
       <c r="D16" s="18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -1320,13 +1330,13 @@
       <c r="B17" s="17"/>
       <c r="C17" s="14"/>
       <c r="D17" s="18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -1340,13 +1350,13 @@
       <c r="B18" s="20"/>
       <c r="C18" s="14"/>
       <c r="D18" s="18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -1360,13 +1370,13 @@
       <c r="B19" s="17"/>
       <c r="C19" s="14"/>
       <c r="D19" s="18" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -1380,13 +1390,13 @@
       <c r="B20" s="20"/>
       <c r="C20" s="14"/>
       <c r="D20" s="18" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -1400,13 +1410,13 @@
       <c r="B21" s="20"/>
       <c r="C21" s="14"/>
       <c r="D21" s="18" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -1420,13 +1430,13 @@
       <c r="B22" s="17"/>
       <c r="C22" s="14"/>
       <c r="D22" s="18" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -1463,7 +1473,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="22" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1613,7 +1623,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="33" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1">
@@ -1621,34 +1631,34 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" customHeight="1">
@@ -1659,31 +1669,31 @@
         <v>45700</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" customHeight="1">
@@ -1694,31 +1704,31 @@
         <v>45700</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" customHeight="1">
@@ -1729,23 +1739,23 @@
         <v>45700</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -1758,23 +1768,23 @@
         <v>45700</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -1787,28 +1797,28 @@
         <v>45700</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -1820,23 +1830,23 @@
         <v>45700</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -1849,24 +1859,24 @@
         <v>45700</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K9" s="6"/>
     </row>
@@ -1878,28 +1888,28 @@
         <v>45700</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="K10" s="6"/>
     </row>
@@ -1911,25 +1921,25 @@
         <v>45700</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -1942,23 +1952,23 @@
         <v>45700</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -1971,23 +1981,23 @@
         <v>45700</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -2000,23 +2010,23 @@
         <v>45700</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -2029,23 +2039,23 @@
         <v>45700</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -2058,23 +2068,23 @@
         <v>45700</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -2087,23 +2097,23 @@
         <v>45700</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -2116,26 +2126,26 @@
         <v>45700</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="K18" s="6"/>
     </row>
@@ -2147,23 +2157,23 @@
         <v>45700</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -2176,28 +2186,28 @@
         <v>45700</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K20" s="6"/>
     </row>
@@ -2209,20 +2219,20 @@
         <v>45700</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -2236,26 +2246,26 @@
         <v>45700</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -2267,16 +2277,16 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -2297,12 +2307,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b556c710-a22d-49cf-9ddd-5d5b9ebc868e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="163e6cfa-b98f-4383-8908-136410dbd9eb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2561,20 +2573,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b556c710-a22d-49cf-9ddd-5d5b9ebc868e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="163e6cfa-b98f-4383-8908-136410dbd9eb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E97845-8BFC-4372-A565-59B68E221017}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FA36966-8DBC-4A7A-A938-9AE9C95376B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b556c710-a22d-49cf-9ddd-5d5b9ebc868e"/>
+    <ds:schemaRef ds:uri="163e6cfa-b98f-4383-8908-136410dbd9eb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2599,12 +2612,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FA36966-8DBC-4A7A-A938-9AE9C95376B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E97845-8BFC-4372-A565-59B68E221017}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b556c710-a22d-49cf-9ddd-5d5b9ebc868e"/>
-    <ds:schemaRef ds:uri="163e6cfa-b98f-4383-8908-136410dbd9eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cải thiện hiển thị cột Description trên nhiều dòng trong ứng dụng và file Excel xuất ra
</commit_message>
<xml_diff>
--- a/public/data/template.xlsx
+++ b/public/data/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\CascadeProjects\excel-mobile-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E34EE9-1E27-4916-9727-67A962DD889B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F503CE-A60E-4016-9684-BEB4884950E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,11 +418,6 @@
     <t>Check cover A/C parking/Storage</t>
   </si>
   <si>
-    <t>Check RAMP to prevent FOD.
-1. Quan sát việc tuân thủ kiểm tra FOD bãi đậu trước khi tàu đáp và sau khi đưa tàu đi của NVKT.
-2. Croscheck tại các bãi có bảo dưỡng lớn xem team bải dưỡng có tuân thủ quy trình ngăn ngừa FOD hay không?</t>
-  </si>
-  <si>
     <t>Check fuel drainage according to the checklist.Random check các tàu thực hiện WKLY có được drain fuel theo WKLY checklist hay không?</t>
   </si>
   <si>
@@ -450,6 +445,11 @@
   </si>
   <si>
     <t>Verify compliance with PTS in operations. PTS là chương trình yêu cầu các đơn vị phải hoàn thành phần việc của mình trong khoảng thời gian CỐ ĐỊNH và TỐI ƯU NHẤT đã được thống nhất bằng văn bản. Nhằm duy trì tổng thời gian dừng/nghỉ giữa các chuyến bay TỐI ƯU.</t>
+  </si>
+  <si>
+    <t>Check RAMP to prevent FOD.
+1. Quan sát việc tuân thủ kiểm tra FOD bãi đậu trước khi tàu đáp và sau khi đưa tàu đi của NVKT.
+2. Croscheck tại các bãi có bảo dưỡng lớn xem team bảo dưỡng có tuân thủ quy trình ngăn ngừa FOD hay không?</t>
   </si>
 </sst>
 </file>
@@ -974,7 +974,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="15"/>
@@ -1033,7 +1033,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>13</v>
@@ -1053,7 +1053,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>13</v>
@@ -1073,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>13</v>
@@ -1133,7 +1133,7 @@
         <v>124</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>13</v>
@@ -1153,7 +1153,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>13</v>
@@ -1173,7 +1173,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>13</v>
@@ -1233,7 +1233,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>26</v>
@@ -1393,7 +1393,7 @@
         <v>42</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>13</v>
@@ -2307,14 +2307,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b556c710-a22d-49cf-9ddd-5d5b9ebc868e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="163e6cfa-b98f-4383-8908-136410dbd9eb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2573,21 +2571,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b556c710-a22d-49cf-9ddd-5d5b9ebc868e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="163e6cfa-b98f-4383-8908-136410dbd9eb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FA36966-8DBC-4A7A-A938-9AE9C95376B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E97845-8BFC-4372-A565-59B68E221017}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b556c710-a22d-49cf-9ddd-5d5b9ebc868e"/>
-    <ds:schemaRef ds:uri="163e6cfa-b98f-4383-8908-136410dbd9eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2612,9 +2609,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62E97845-8BFC-4372-A565-59B68E221017}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FA36966-8DBC-4A7A-A938-9AE9C95376B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b556c710-a22d-49cf-9ddd-5d5b9ebc868e"/>
+    <ds:schemaRef ds:uri="163e6cfa-b98f-4383-8908-136410dbd9eb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>